<commit_message>
personal tracker updated for day one
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -39,6 +39,12 @@
   <si>
     <t xml:space="preserve">Jumping Jacks</t>
   </si>
+  <si>
+    <t xml:space="preserve">Squats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curling</t>
+  </si>
 </sst>
 </file>
 
@@ -53,6 +59,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -138,16 +145,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -170,6 +177,12 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -177,6 +190,24 @@
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day two
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Curling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 min</t>
   </si>
 </sst>
 </file>
@@ -148,13 +151,13 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -216,6 +219,24 @@
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day three
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -46,7 +46,13 @@
     <t xml:space="preserve">Curling</t>
   </si>
   <si>
+    <t xml:space="preserve">Sides</t>
+  </si>
+  <si>
     <t xml:space="preserve">2 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 min</t>
   </si>
 </sst>
 </file>
@@ -148,10 +154,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -186,6 +192,9 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -227,7 +236,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>20</v>
@@ -245,6 +254,27 @@
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day four
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -284,6 +284,27 @@
       <c r="B5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day five
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -157,7 +157,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -313,6 +313,27 @@
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day six
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -157,7 +157,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6:I6"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,6 +342,27 @@
       <c r="B7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day seven
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -157,7 +157,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -371,6 +371,27 @@
       <c r="B8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day eight
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -157,7 +157,7 @@
   <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -400,6 +400,27 @@
       <c r="B9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day nine
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Days</t>
   </si>
   <si>
-    <t xml:space="preserve">Swimming</t>
+    <t xml:space="preserve">Breast Stroke Drill</t>
   </si>
   <si>
     <t xml:space="preserve">Push Ups</t>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Sides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seiza (Japanese Sitting Posture)</t>
   </si>
   <si>
     <t xml:space="preserve">2 min</t>
@@ -154,17 +157,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -195,6 +202,9 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -236,7 +246,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>20</v>
@@ -262,7 +272,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>20</v>
@@ -372,7 +382,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>0</v>
@@ -387,7 +397,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>0</v>
@@ -428,6 +438,27 @@
       </c>
       <c r="B10" s="0" t="n">
         <v>9</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day ten
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,6 +474,21 @@
       <c r="B11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day eleven
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,9 +474,15 @@
       <c r="B11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="D11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="F11" s="0" t="n">
         <v>20</v>
       </c>
@@ -487,7 +493,10 @@
         <v>20</v>
       </c>
       <c r="I11" s="0" t="n">
-        <v>20</v>
+        <v>40</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,6 +505,30 @@
       </c>
       <c r="B12" s="0" t="n">
         <v>11</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day twelve
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,8 +527,8 @@
       <c r="I12" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="J12" s="0" t="n">
-        <v>0</v>
+      <c r="J12" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,6 +537,30 @@
       </c>
       <c r="B13" s="0" t="n">
         <v>12</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day thirteen
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -570,6 +570,21 @@
       <c r="B14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day-14
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,6 +593,15 @@
       <c r="B15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day-15
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -610,6 +610,15 @@
       <c r="B16" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day-16
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,6 +627,15 @@
       <c r="B17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day-18
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -145,12 +145,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -661,6 +661,15 @@
       <c r="B19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">

</xml_diff>

<commit_message>
personal tracker updated for day-20
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -662,13 +662,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I19" s="0" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,6 +678,15 @@
       <c r="B20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -685,6 +694,15 @@
       </c>
       <c r="B21" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
personal tracker updated for day-21
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -712,6 +712,18 @@
       <c r="B22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">

</xml_diff>

<commit_message>
tracker updated for day-23
</commit_message>
<xml_diff>
--- a/Personal/Tracker.xlsx
+++ b/Personal/Tracker.xlsx
@@ -163,7 +163,7 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -732,6 +732,18 @@
       <c r="B23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="C23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">

</xml_diff>